<commit_message>
Partial Output and predictions. There may be something interesting here.
</commit_message>
<xml_diff>
--- a/NumberChain/CalculatedResults.xlsx
+++ b/NumberChain/CalculatedResults.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xavier V\Source\Repos\pythonexperiments\NumberChain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xavi\Source\Repos\pythonexperiments\NumberChain\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17067" windowHeight="8180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17070" windowHeight="8175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,22 +24,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Size</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Solution Size</t>
   </si>
   <si>
-    <t>Excluded Primes</t>
+    <t>Problem Size</t>
+  </si>
+  <si>
+    <t>Unique Solutions</t>
+  </si>
+  <si>
+    <t>Start Value</t>
+  </si>
+  <si>
+    <t>End Value</t>
+  </si>
+  <si>
+    <t>Largest Start</t>
+  </si>
+  <si>
+    <t>Largest End</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,13 +59,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,13 +89,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,31 +411,1391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.64453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>44</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>88</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>96</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>112</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>352</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>11</v>
+      </c>
+      <c r="F22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>448</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>448</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>11</v>
+      </c>
+      <c r="F24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>13</v>
+      </c>
+      <c r="F25" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>23</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>24</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>26</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>26</v>
+      </c>
+      <c r="D32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>27</v>
+      </c>
+      <c r="D33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>28</v>
+      </c>
+      <c r="D34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>29</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>31</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>31</v>
+      </c>
+      <c r="D38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>32</v>
+      </c>
+      <c r="D39">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>33</v>
+      </c>
+      <c r="D40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>34</v>
+      </c>
+      <c r="D41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>34</v>
+      </c>
+      <c r="D42">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>36</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>36</v>
+      </c>
+      <c r="D44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>37</v>
+      </c>
+      <c r="D45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>38</v>
+      </c>
+      <c r="D46">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>39</v>
+      </c>
+      <c r="D47">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>39</v>
+      </c>
+      <c r="D48">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>41</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>41</v>
+      </c>
+      <c r="D50">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>42</v>
+      </c>
+      <c r="D51">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>43</v>
+      </c>
+      <c r="D52">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>44</v>
+      </c>
+      <c r="D53">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>44</v>
+      </c>
+      <c r="D54">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>46</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>46</v>
+      </c>
+      <c r="D56">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>47</v>
+      </c>
+      <c r="D57">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>48</v>
+      </c>
+      <c r="D58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>49</v>
+      </c>
+      <c r="D59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>49</v>
+      </c>
+      <c r="D60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>51</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>51</v>
+      </c>
+      <c r="D62">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>52</v>
+      </c>
+      <c r="D63">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>53</v>
+      </c>
+      <c r="D64">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>54</v>
+      </c>
+      <c r="D65">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>54</v>
+      </c>
+      <c r="D66">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>56</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>56</v>
+      </c>
+      <c r="D68">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>57</v>
+      </c>
+      <c r="D69">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>58</v>
+      </c>
+      <c r="D70">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>59</v>
+      </c>
+      <c r="D71">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>59</v>
+      </c>
+      <c r="D72">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>61</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>61</v>
+      </c>
+      <c r="D74">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>62</v>
+      </c>
+      <c r="D75">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>63</v>
+      </c>
+      <c r="D76">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>64</v>
+      </c>
+      <c r="D77">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>64</v>
+      </c>
+      <c r="D78">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>66</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>66</v>
+      </c>
+      <c r="D80">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>67</v>
+      </c>
+      <c r="D81">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>68</v>
+      </c>
+      <c r="D82">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>69</v>
+      </c>
+      <c r="D83">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>69</v>
+      </c>
+      <c r="D84">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>71</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>71</v>
+      </c>
+      <c r="D86">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>72</v>
+      </c>
+      <c r="D87">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>73</v>
+      </c>
+      <c r="D88">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>74</v>
+      </c>
+      <c r="D89">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>74</v>
+      </c>
+      <c r="D90">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>76</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>76</v>
+      </c>
+      <c r="D92">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>77</v>
+      </c>
+      <c r="D93">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>78</v>
+      </c>
+      <c r="D94">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>79</v>
+      </c>
+      <c r="D95">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>79</v>
+      </c>
+      <c r="D96">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>81</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>81</v>
+      </c>
+      <c r="D98">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>82</v>
+      </c>
+      <c r="D99">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>83</v>
+      </c>
+      <c r="D100">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>84</v>
+      </c>
+      <c r="D101">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>